<commit_message>
mod updates, prep for tech and abyss
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74CCE2F-8E55-4FD0-BF06-4B512AE9CAB2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A564E59-5CFD-497D-BFEA-3D219BF2899E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{D4271B40-E291-4F7D-B212-DFF8B5827327}"/>
   </bookViews>
@@ -5753,8 +5753,8 @@
   </sheetPr>
   <dimension ref="A1:N136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2.1.1 changes + banner images
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\Craft-to-Exile-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241832F4-4F02-484B-9EFA-FE2189EB8A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79039AC-22EF-42FD-AE8D-7DD106F07648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D4271B40-E291-4F7D-B212-DFF8B5827327}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="936">
   <si>
     <t>armor_percent</t>
   </si>
@@ -2840,6 +2840,9 @@
   </si>
   <si>
     <t>low_armor_flat</t>
+  </si>
+  <si>
+    <t>blaze_bow</t>
   </si>
 </sst>
 </file>
@@ -2911,19 +2914,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3255,31 +3257,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -4382,28 +4384,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -4423,28 +4425,28 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>10000</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>20</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>2</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>580</v>
       </c>
       <c r="I2" t="s">
@@ -4452,28 +4454,28 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
         <v>10000</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>20</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>808</v>
       </c>
       <c r="I3" t="s">
@@ -4481,28 +4483,28 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
         <v>10000</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>20</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>582</v>
       </c>
       <c r="I4" t="s">
@@ -4510,28 +4512,28 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>10000</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>25</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>3</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>812</v>
       </c>
       <c r="I5" t="s">
@@ -4542,28 +4544,28 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>614</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
         <v>10000</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>30</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>2</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>597</v>
       </c>
       <c r="I6" t="s">
@@ -4571,28 +4573,28 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
         <v>10000</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>35</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>2</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>597</v>
       </c>
       <c r="I7" t="s">
@@ -4612,10 +4614,10 @@
       <c r="D8">
         <v>10000</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>99</v>
       </c>
       <c r="G8">
@@ -4629,28 +4631,28 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>593</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0</v>
       </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
         <v>10000</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>10</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>30</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>3</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>591</v>
       </c>
       <c r="I9" t="s">
@@ -4661,28 +4663,28 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0</v>
       </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>10000</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>10</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>30</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>3</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>591</v>
       </c>
       <c r="I10" t="s">
@@ -4693,40 +4695,40 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0</v>
       </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>10000</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>10</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>30</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>3</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4741,28 +4743,28 @@
       <c r="D12">
         <v>10000</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>10</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>30</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>3</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -4777,10 +4779,10 @@
       <c r="D13" s="4">
         <v>10000</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>10</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>40</v>
       </c>
       <c r="G13" s="4">
@@ -4811,30 +4813,30 @@
       <c r="D14" s="3">
         <v>10000</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>10</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>60</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>4</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>866</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="8"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -4849,30 +4851,30 @@
       <c r="D15" s="3">
         <v>10000</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>15</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>50</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>4</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>808</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="9" t="s">
+      <c r="J15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="L15" s="8"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -4887,30 +4889,30 @@
       <c r="D16" s="3">
         <v>10000</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>15</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>50</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>4</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>809</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -4925,30 +4927,30 @@
       <c r="D17" s="3">
         <v>10000</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>15</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>50</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>4</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4963,68 +4965,68 @@
       <c r="D18">
         <v>10000</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>25</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>50</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>4</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>604</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>0</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>2500</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>30</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>99</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>4</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -5039,30 +5041,30 @@
       <c r="D20">
         <v>10000</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>35</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>70</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>4</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -5077,30 +5079,30 @@
       <c r="D21">
         <v>10000</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>35</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>70</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>4</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -5109,34 +5111,34 @@
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>2500</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>40</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>99</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>3</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -5145,36 +5147,36 @@
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>3</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>250</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>40</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>99</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>4</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -5189,10 +5191,10 @@
       <c r="D24" s="4">
         <v>50</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>45</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>99</v>
       </c>
       <c r="G24" s="4">
@@ -5221,32 +5223,32 @@
       <c r="B25">
         <v>0</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>4</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>50</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>45</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>99</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>2</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -5261,30 +5263,30 @@
       <c r="D26">
         <v>10000</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>50</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>99</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>4</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="J26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="K26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -5293,36 +5295,36 @@
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27" s="6">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6">
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
         <v>10000</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>50</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>99</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>3</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="J27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -5331,38 +5333,38 @@
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>3</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>250</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>50</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>99</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>5</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J28" s="6" t="s">
+      <c r="I28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K28" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="L28" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -5371,36 +5373,36 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29" s="6">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
         <v>10000</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>50</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>99</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>4</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -5409,32 +5411,32 @@
       <c r="B30" s="3">
         <v>0</v>
       </c>
-      <c r="C30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8">
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
         <v>200555</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <v>50</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>99</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <v>2</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>619</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -5443,34 +5445,34 @@
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>4</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>50</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>70</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>99</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>3</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -5479,40 +5481,40 @@
       <c r="B32" s="3">
         <v>0</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <v>4</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <v>50</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>70</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>99</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <v>6</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>874</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="M32" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="N32" s="6"/>
+      <c r="N32" s="5"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -5521,40 +5523,40 @@
       <c r="B33" s="3">
         <v>0</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>4</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <v>50</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>70</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>99</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="7">
         <v>6</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="7" t="s">
         <v>875</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="K33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L33" s="8" t="s">
+      <c r="L33" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="M33" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="N33" s="6"/>
+      <c r="N33" s="5"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -5563,40 +5565,40 @@
       <c r="B34" s="3">
         <v>0</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>4</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <v>50</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>70</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <v>99</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="7">
         <v>6</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="7" t="s">
         <v>873</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="7" t="s">
         <v>871</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="L34" s="8" t="s">
+      <c r="L34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M34" s="8" t="s">
+      <c r="M34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N34" s="6"/>
+      <c r="N34" s="5"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -5605,34 +5607,34 @@
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="C35" s="6">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6">
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
         <v>10000</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>85</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <v>99</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="5">
         <v>3</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J35" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -5647,30 +5649,30 @@
       <c r="D36">
         <v>50</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>90</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <v>99</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="5">
         <v>4</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -5685,10 +5687,10 @@
       <c r="D37">
         <v>50</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <v>90</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="5">
         <v>99</v>
       </c>
       <c r="G37">
@@ -5720,10 +5722,10 @@
       <c r="D38">
         <v>50</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>90</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <v>99</v>
       </c>
       <c r="G38">
@@ -5749,25 +5751,25 @@
       <c r="B39">
         <v>0</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <v>4</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>50</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>90</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <v>99</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="5">
         <v>4</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="5" t="s">
         <v>355</v>
       </c>
       <c r="J39" t="s">
@@ -5825,10 +5827,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:N149"/>
+  <dimension ref="A1:N151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="H129" sqref="H129"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5839,43 +5841,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>628</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
         <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -5889,7 +5891,7 @@
       <c r="B2" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="3">
@@ -5924,7 +5926,7 @@
       <c r="B3" s="4" t="s">
         <v>816</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="4">
@@ -5959,7 +5961,7 @@
       <c r="B4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>3</v>
       </c>
       <c r="D4" s="3">
@@ -5996,7 +5998,7 @@
       <c r="B5" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
       <c r="D5" s="4">
@@ -6033,7 +6035,7 @@
       <c r="B6" s="4" t="s">
         <v>867</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>4</v>
       </c>
       <c r="D6" s="4">
@@ -6055,7 +6057,7 @@
       <c r="J6" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>483</v>
       </c>
       <c r="L6" s="3"/>
@@ -6070,7 +6072,7 @@
       <c r="B7" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>5</v>
       </c>
       <c r="D7" s="3">
@@ -6107,7 +6109,7 @@
       <c r="B8" s="4" t="s">
         <v>868</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="4">
@@ -6142,7 +6144,7 @@
       <c r="B9" s="4" t="s">
         <v>818</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>2</v>
       </c>
       <c r="D9" s="4">
@@ -6179,7 +6181,7 @@
       <c r="B10" s="4" t="s">
         <v>819</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>2</v>
       </c>
       <c r="D10" s="4">
@@ -6214,7 +6216,7 @@
       <c r="B11" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>3</v>
       </c>
       <c r="D11" s="3">
@@ -6249,7 +6251,7 @@
       <c r="B12" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
       <c r="D12" s="3">
@@ -6284,7 +6286,7 @@
       <c r="B13" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>3</v>
       </c>
       <c r="D13" s="3">
@@ -6319,7 +6321,7 @@
       <c r="B14" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>3</v>
       </c>
       <c r="D14" s="3">
@@ -6354,7 +6356,7 @@
       <c r="B15" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>4</v>
       </c>
       <c r="D15" s="4">
@@ -6378,7 +6380,7 @@
       <c r="J15" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>483</v>
       </c>
       <c r="L15" s="3"/>
@@ -6393,7 +6395,7 @@
       <c r="B16" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="3">
@@ -6427,7 +6429,7 @@
       <c r="A17" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>913</v>
       </c>
       <c r="C17" s="3">
@@ -6465,7 +6467,7 @@
       <c r="B18" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>2</v>
       </c>
       <c r="D18" s="3">
@@ -6500,7 +6502,7 @@
       <c r="B19" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>3</v>
       </c>
       <c r="D19" s="3">
@@ -6535,7 +6537,7 @@
       <c r="B20" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>3</v>
       </c>
       <c r="D20" s="3">
@@ -6573,7 +6575,7 @@
       <c r="B21" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>4</v>
       </c>
       <c r="D21" s="3">
@@ -6604,7 +6606,7 @@
       <c r="B22" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>4</v>
       </c>
       <c r="D22" s="3">
@@ -6638,16 +6640,16 @@
       <c r="A23" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>910</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>5</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>4</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -6678,7 +6680,7 @@
       <c r="B24" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>4</v>
       </c>
       <c r="D24" s="3">
@@ -6713,7 +6715,7 @@
       <c r="B25" s="3" t="s">
         <v>656</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>4</v>
       </c>
       <c r="D25" s="3">
@@ -6748,7 +6750,7 @@
       <c r="B26" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>4</v>
       </c>
       <c r="D26" s="3">
@@ -6785,7 +6787,7 @@
       <c r="B27" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>4</v>
       </c>
       <c r="D27" s="3">
@@ -6820,7 +6822,7 @@
       <c r="B28" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>2</v>
       </c>
       <c r="D28" s="3">
@@ -6857,7 +6859,7 @@
       <c r="B29" s="3" t="s">
         <v>664</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>2</v>
       </c>
       <c r="D29" s="3">
@@ -6894,10 +6896,10 @@
       <c r="B30" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>2</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>1</v>
       </c>
       <c r="E30" s="3">
@@ -6931,10 +6933,10 @@
       <c r="B31" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>2</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="E31" s="3">
@@ -6968,10 +6970,10 @@
       <c r="B32" s="4" t="s">
         <v>823</v>
       </c>
-      <c r="C32" s="8">
-        <v>1</v>
-      </c>
-      <c r="D32" s="9">
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8">
         <v>1</v>
       </c>
       <c r="E32" s="4">
@@ -7001,10 +7003,10 @@
       <c r="B33" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>2</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="8">
         <v>1</v>
       </c>
       <c r="E33" s="4">
@@ -7036,10 +7038,10 @@
       <c r="B34" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>3</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <v>1</v>
       </c>
       <c r="E34" s="3">
@@ -7070,16 +7072,16 @@
       <c r="A35" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>881</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>4</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="7">
         <v>3</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>250</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -7110,10 +7112,10 @@
       <c r="B36" s="4" t="s">
         <v>822</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>5</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="8">
         <v>4</v>
       </c>
       <c r="E36" s="4">
@@ -7292,10 +7294,10 @@
       <c r="B41" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <v>5</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="7">
         <v>1</v>
       </c>
       <c r="E41" s="3">
@@ -7327,7 +7329,7 @@
       <c r="B42" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="7">
         <v>1</v>
       </c>
       <c r="D42" s="4">
@@ -7504,7 +7506,7 @@
       <c r="B47" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="7">
         <v>2</v>
       </c>
       <c r="D47" s="3">
@@ -7539,7 +7541,7 @@
       <c r="B48" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="7">
         <v>3</v>
       </c>
       <c r="D48" s="3">
@@ -7574,7 +7576,7 @@
       <c r="B49" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="7">
         <v>4</v>
       </c>
       <c r="D49" s="4">
@@ -7611,7 +7613,7 @@
       <c r="B50" s="4" t="s">
         <v>829</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="7">
         <v>5</v>
       </c>
       <c r="D50" s="4">
@@ -7648,7 +7650,7 @@
       <c r="B51" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="7">
         <v>1</v>
       </c>
       <c r="D51" s="4">
@@ -7685,7 +7687,7 @@
       <c r="B52" s="4" t="s">
         <v>832</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="7">
         <v>2</v>
       </c>
       <c r="D52" s="4">
@@ -7720,7 +7722,7 @@
       <c r="B53" s="4" t="s">
         <v>831</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="7">
         <v>3</v>
       </c>
       <c r="D53" s="4">
@@ -7757,7 +7759,7 @@
       <c r="B54" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="7">
         <v>1</v>
       </c>
       <c r="D54" s="4">
@@ -7789,16 +7791,16 @@
       <c r="A55" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>888</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="7">
         <v>2</v>
       </c>
-      <c r="D55" s="8">
-        <v>1</v>
-      </c>
-      <c r="E55" s="8">
+      <c r="D55" s="7">
+        <v>1</v>
+      </c>
+      <c r="E55" s="7">
         <v>10000</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -7827,7 +7829,7 @@
       <c r="B56" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="7">
         <v>4</v>
       </c>
       <c r="D56" s="3">
@@ -7863,16 +7865,16 @@
       <c r="A57" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>909</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="8">
         <v>5</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="8">
         <v>4</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="8">
         <v>50</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -7903,7 +7905,7 @@
       <c r="B58" s="4" t="s">
         <v>837</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C58" s="7">
         <v>1</v>
       </c>
       <c r="D58" s="4">
@@ -7936,7 +7938,7 @@
       <c r="B59" s="4" t="s">
         <v>838</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C59" s="7">
         <v>1</v>
       </c>
       <c r="D59" s="4">
@@ -7973,7 +7975,7 @@
       <c r="B60" s="4" t="s">
         <v>836</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C60" s="7">
         <v>2</v>
       </c>
       <c r="D60" s="4">
@@ -8010,7 +8012,7 @@
       <c r="B61" s="4" t="s">
         <v>839</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C61" s="7">
         <v>3</v>
       </c>
       <c r="D61" s="4">
@@ -8045,29 +8047,29 @@
       <c r="B62" s="3" t="s">
         <v>702</v>
       </c>
-      <c r="C62" s="9">
-        <v>1</v>
-      </c>
-      <c r="D62" s="9">
+      <c r="C62" s="8">
+        <v>1</v>
+      </c>
+      <c r="D62" s="8">
         <v>3</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="8">
         <v>250</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9" t="s">
+      <c r="G62" s="8"/>
+      <c r="H62" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="I62" s="9" t="s">
+      <c r="I62" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J62" s="9" t="s">
+      <c r="J62" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K62" s="9"/>
+      <c r="K62" s="8"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3" t="s">
         <v>703</v>
@@ -8083,29 +8085,29 @@
       <c r="B63" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="C63" s="9">
-        <v>1</v>
-      </c>
-      <c r="D63" s="9">
+      <c r="C63" s="8">
+        <v>1</v>
+      </c>
+      <c r="D63" s="8">
         <v>3</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="8">
         <v>250</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F63" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9" t="s">
+      <c r="G63" s="8"/>
+      <c r="H63" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I63" s="9" t="s">
+      <c r="I63" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="J63" s="9" t="s">
+      <c r="J63" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K63" s="9" t="s">
+      <c r="K63" s="8" t="s">
         <v>28</v>
       </c>
       <c r="L63" s="3"/>
@@ -8117,16 +8119,16 @@
       <c r="A64" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>896</v>
       </c>
-      <c r="C64" s="8">
-        <v>1</v>
-      </c>
-      <c r="D64" s="8">
-        <v>1</v>
-      </c>
-      <c r="E64" s="8">
+      <c r="C64" s="7">
+        <v>1</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7">
         <v>10000</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -8155,7 +8157,7 @@
       <c r="B65" s="3" t="s">
         <v>691</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="7">
         <v>2</v>
       </c>
       <c r="D65" s="3">
@@ -8192,29 +8194,29 @@
       <c r="B66" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8">
         <v>2</v>
       </c>
-      <c r="D66" s="9">
-        <v>1</v>
-      </c>
-      <c r="E66" s="9">
+      <c r="D66" s="8">
+        <v>1</v>
+      </c>
+      <c r="E66" s="8">
         <v>10000</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9" t="s">
+      <c r="G66" s="8"/>
+      <c r="H66" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I66" s="9" t="s">
+      <c r="I66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J66" s="9" t="s">
+      <c r="J66" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K66" s="9" t="s">
+      <c r="K66" s="8" t="s">
         <v>386</v>
       </c>
       <c r="L66" s="3" t="s">
@@ -8231,29 +8233,29 @@
       <c r="B67" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8">
         <v>2</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="8">
         <v>3</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E67" s="8">
         <v>250</v>
       </c>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9" t="s">
+      <c r="G67" s="8"/>
+      <c r="H67" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="I67" s="9" t="s">
+      <c r="I67" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="J67" s="9" t="s">
+      <c r="J67" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="K67" s="9"/>
+      <c r="K67" s="8"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3" t="s">
         <v>705</v>
@@ -8263,16 +8265,16 @@
       <c r="A68" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="7" t="s">
         <v>903</v>
       </c>
-      <c r="C68" s="8">
+      <c r="C68" s="7">
         <v>2</v>
       </c>
-      <c r="D68" s="8">
+      <c r="D68" s="7">
         <v>4</v>
       </c>
-      <c r="E68" s="8">
+      <c r="E68" s="7">
         <v>50</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -8297,25 +8299,25 @@
       <c r="B69" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <v>3</v>
       </c>
-      <c r="D69" s="9">
-        <v>1</v>
-      </c>
-      <c r="E69" s="9">
+      <c r="D69" s="8">
+        <v>1</v>
+      </c>
+      <c r="E69" s="8">
         <v>10000</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9" t="s">
+      <c r="G69" s="8"/>
+      <c r="H69" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3" t="s">
         <v>694</v>
@@ -8328,29 +8330,29 @@
       <c r="B70" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C70" s="8">
         <v>3</v>
       </c>
-      <c r="D70" s="9">
-        <v>1</v>
-      </c>
-      <c r="E70" s="9">
+      <c r="D70" s="8">
+        <v>1</v>
+      </c>
+      <c r="E70" s="8">
         <v>10000</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9" t="s">
+      <c r="G70" s="8"/>
+      <c r="H70" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="I70" s="9" t="s">
+      <c r="I70" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="J70" s="9" t="s">
+      <c r="J70" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="K70" s="9" t="s">
+      <c r="K70" s="8" t="s">
         <v>712</v>
       </c>
       <c r="L70" s="3"/>
@@ -8365,29 +8367,29 @@
       <c r="B71" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="C71" s="9">
+      <c r="C71" s="8">
         <v>4</v>
       </c>
-      <c r="D71" s="9">
-        <v>1</v>
-      </c>
-      <c r="E71" s="9">
+      <c r="D71" s="8">
+        <v>1</v>
+      </c>
+      <c r="E71" s="8">
         <v>10000</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9" t="s">
+      <c r="G71" s="8"/>
+      <c r="H71" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="I71" s="9" t="s">
+      <c r="I71" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J71" s="9" t="s">
+      <c r="J71" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K71" s="9"/>
+      <c r="K71" s="8"/>
       <c r="L71" s="3"/>
       <c r="M71" s="3" t="s">
         <v>709</v>
@@ -8400,7 +8402,7 @@
       <c r="B72" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="C72" s="8">
+      <c r="C72" s="7">
         <v>5</v>
       </c>
       <c r="D72" s="3">
@@ -8435,29 +8437,29 @@
       <c r="B73" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C73" s="8">
         <v>5</v>
       </c>
-      <c r="D73" s="9">
-        <v>1</v>
-      </c>
-      <c r="E73" s="9">
+      <c r="D73" s="8">
+        <v>1</v>
+      </c>
+      <c r="E73" s="8">
         <v>10000</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F73" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9" t="s">
+      <c r="G73" s="8"/>
+      <c r="H73" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="I73" s="9" t="s">
+      <c r="I73" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="J73" s="9" t="s">
+      <c r="J73" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K73" s="9"/>
+      <c r="K73" s="8"/>
       <c r="L73" s="3"/>
       <c r="M73" s="3" t="s">
         <v>696</v>
@@ -8470,31 +8472,31 @@
       <c r="B74" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C74" s="8">
         <v>5</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="8">
         <v>4</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E74" s="8">
         <v>50</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F74" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G74" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="H74" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="I74" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="J74" s="9" t="s">
+      <c r="J74" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="K74" s="9" t="s">
+      <c r="K74" s="8" t="s">
         <v>384</v>
       </c>
       <c r="L74" s="3"/>
@@ -8509,27 +8511,27 @@
       <c r="B75" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="C75" s="9">
-        <v>1</v>
-      </c>
-      <c r="D75" s="9">
-        <v>1</v>
-      </c>
-      <c r="E75" s="9">
+      <c r="C75" s="8">
+        <v>1</v>
+      </c>
+      <c r="D75" s="8">
+        <v>1</v>
+      </c>
+      <c r="E75" s="8">
         <v>10000</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9" t="s">
+      <c r="G75" s="8"/>
+      <c r="H75" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="I75" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
+      <c r="I75" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
       <c r="L75" s="3"/>
       <c r="M75" s="3" t="s">
         <v>722</v>
@@ -8542,29 +8544,29 @@
       <c r="B76" s="3" t="s">
         <v>715</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="8">
         <v>2</v>
       </c>
-      <c r="D76" s="9">
-        <v>1</v>
-      </c>
-      <c r="E76" s="9">
+      <c r="D76" s="8">
+        <v>1</v>
+      </c>
+      <c r="E76" s="8">
         <v>10000</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9" t="s">
+      <c r="G76" s="8"/>
+      <c r="H76" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="I76" s="9" t="s">
+      <c r="I76" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="J76" s="9" t="s">
+      <c r="J76" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K76" s="9"/>
+      <c r="K76" s="8"/>
       <c r="L76" s="3"/>
       <c r="M76" s="3" t="s">
         <v>648</v>
@@ -8577,29 +8579,29 @@
       <c r="B77" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="C77" s="9">
+      <c r="C77" s="8">
         <v>2</v>
       </c>
-      <c r="D77" s="9">
-        <v>1</v>
-      </c>
-      <c r="E77" s="9">
+      <c r="D77" s="8">
+        <v>1</v>
+      </c>
+      <c r="E77" s="8">
         <v>10000</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9" t="s">
+      <c r="G77" s="8"/>
+      <c r="H77" s="8" t="s">
         <v>721</v>
       </c>
-      <c r="I77" s="9" t="s">
+      <c r="I77" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="J77" s="9" t="s">
+      <c r="J77" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="K77" s="9"/>
+      <c r="K77" s="8"/>
       <c r="L77" s="3"/>
       <c r="M77" s="3" t="s">
         <v>622</v>
@@ -8612,29 +8614,29 @@
       <c r="B78" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C78" s="8">
         <v>3</v>
       </c>
-      <c r="D78" s="9">
-        <v>1</v>
-      </c>
-      <c r="E78" s="9">
+      <c r="D78" s="8">
+        <v>1</v>
+      </c>
+      <c r="E78" s="8">
         <v>10000</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9" t="s">
+      <c r="G78" s="8"/>
+      <c r="H78" s="8" t="s">
         <v>719</v>
       </c>
-      <c r="I78" s="9" t="s">
+      <c r="I78" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="J78" s="9" t="s">
+      <c r="J78" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="K78" s="9"/>
+      <c r="K78" s="8"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3" t="s">
         <v>720</v>
@@ -8644,16 +8646,16 @@
       <c r="A79" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="7" t="s">
         <v>892</v>
       </c>
-      <c r="C79" s="8">
-        <v>1</v>
-      </c>
-      <c r="D79" s="8">
-        <v>1</v>
-      </c>
-      <c r="E79" s="8">
+      <c r="C79" s="7">
+        <v>1</v>
+      </c>
+      <c r="D79" s="7">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7">
         <v>10000</v>
       </c>
       <c r="F79" s="3" t="s">
@@ -8684,29 +8686,29 @@
       <c r="B80" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="C80" s="9">
+      <c r="C80" s="8">
         <v>2</v>
       </c>
-      <c r="D80" s="9">
-        <v>1</v>
-      </c>
-      <c r="E80" s="9">
+      <c r="D80" s="8">
+        <v>1</v>
+      </c>
+      <c r="E80" s="8">
         <v>10000</v>
       </c>
-      <c r="F80" s="9" t="s">
+      <c r="F80" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9" t="s">
+      <c r="G80" s="8"/>
+      <c r="H80" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I80" s="9" t="s">
+      <c r="I80" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J80" s="9" t="s">
+      <c r="J80" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="K80" s="9"/>
+      <c r="K80" s="8"/>
       <c r="L80" s="3"/>
       <c r="M80" s="3" t="s">
         <v>713</v>
@@ -8719,29 +8721,29 @@
       <c r="B81" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="C81" s="9">
+      <c r="C81" s="8">
         <v>2</v>
       </c>
-      <c r="D81" s="9">
-        <v>1</v>
-      </c>
-      <c r="E81" s="9">
+      <c r="D81" s="8">
+        <v>1</v>
+      </c>
+      <c r="E81" s="8">
         <v>10000</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9" t="s">
+      <c r="G81" s="8"/>
+      <c r="H81" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="I81" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J81" s="9" t="s">
+      <c r="I81" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J81" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="K81" s="9"/>
+      <c r="K81" s="8"/>
       <c r="L81" s="3"/>
       <c r="M81" s="3" t="s">
         <v>692</v>
@@ -8754,29 +8756,29 @@
       <c r="B82" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="C82" s="9">
+      <c r="C82" s="8">
         <v>2</v>
       </c>
-      <c r="D82" s="9">
-        <v>1</v>
-      </c>
-      <c r="E82" s="9">
+      <c r="D82" s="8">
+        <v>1</v>
+      </c>
+      <c r="E82" s="8">
         <v>10000</v>
       </c>
-      <c r="F82" s="9" t="s">
+      <c r="F82" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9" t="s">
+      <c r="G82" s="8"/>
+      <c r="H82" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I82" s="9" t="s">
+      <c r="I82" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J82" s="9" t="s">
+      <c r="J82" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="K82" s="9"/>
+      <c r="K82" s="8"/>
       <c r="L82" s="3"/>
       <c r="M82" s="3" t="s">
         <v>713</v>
@@ -8789,29 +8791,29 @@
       <c r="B83" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C83" s="8">
         <v>2</v>
       </c>
-      <c r="D83" s="9">
-        <v>1</v>
-      </c>
-      <c r="E83" s="9">
+      <c r="D83" s="8">
+        <v>1</v>
+      </c>
+      <c r="E83" s="8">
         <v>10000</v>
       </c>
-      <c r="F83" s="9" t="s">
+      <c r="F83" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9" t="s">
+      <c r="G83" s="8"/>
+      <c r="H83" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="I83" s="9" t="s">
+      <c r="I83" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J83" s="9" t="s">
+      <c r="J83" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="K83" s="9"/>
+      <c r="K83" s="8"/>
       <c r="L83" s="3"/>
       <c r="M83" s="3" t="s">
         <v>713</v>
@@ -8821,16 +8823,16 @@
       <c r="A84" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="7" t="s">
         <v>895</v>
       </c>
-      <c r="C84" s="8">
+      <c r="C84" s="7">
         <v>2</v>
       </c>
-      <c r="D84" s="8">
-        <v>1</v>
-      </c>
-      <c r="E84" s="8">
+      <c r="D84" s="7">
+        <v>1</v>
+      </c>
+      <c r="E84" s="7">
         <v>10000</v>
       </c>
       <c r="F84" s="3" t="s">
@@ -8856,16 +8858,16 @@
       <c r="A85" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="7" t="s">
         <v>894</v>
       </c>
-      <c r="C85" s="8">
+      <c r="C85" s="7">
         <v>3</v>
       </c>
-      <c r="D85" s="8">
+      <c r="D85" s="7">
         <v>3</v>
       </c>
-      <c r="E85" s="8">
+      <c r="E85" s="7">
         <v>250</v>
       </c>
       <c r="F85" s="3" t="s">
@@ -8898,29 +8900,29 @@
       <c r="B86" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C86" s="8">
         <v>2</v>
       </c>
-      <c r="D86" s="9">
-        <v>1</v>
-      </c>
-      <c r="E86" s="9">
+      <c r="D86" s="8">
+        <v>1</v>
+      </c>
+      <c r="E86" s="8">
         <v>10000</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F86" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9" t="s">
+      <c r="G86" s="8"/>
+      <c r="H86" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="I86" s="9" t="s">
+      <c r="I86" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J86" s="9" t="s">
+      <c r="J86" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K86" s="9"/>
+      <c r="K86" s="8"/>
       <c r="L86" s="3"/>
       <c r="M86" s="3" t="s">
         <v>670</v>
@@ -8933,29 +8935,29 @@
       <c r="B87" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C87" s="8">
         <v>3</v>
       </c>
-      <c r="D87" s="9">
-        <v>1</v>
-      </c>
-      <c r="E87" s="9">
+      <c r="D87" s="8">
+        <v>1</v>
+      </c>
+      <c r="E87" s="8">
         <v>10000</v>
       </c>
-      <c r="F87" s="9" t="s">
+      <c r="F87" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9" t="s">
+      <c r="G87" s="8"/>
+      <c r="H87" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I87" s="9" t="s">
+      <c r="I87" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J87" s="9" t="s">
+      <c r="J87" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K87" s="9"/>
+      <c r="K87" s="8"/>
       <c r="L87" s="3"/>
       <c r="M87" s="3" t="s">
         <v>733</v>
@@ -8968,29 +8970,29 @@
       <c r="B88" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C88" s="8">
         <v>4</v>
       </c>
-      <c r="D88" s="9">
-        <v>1</v>
-      </c>
-      <c r="E88" s="9">
+      <c r="D88" s="8">
+        <v>1</v>
+      </c>
+      <c r="E88" s="8">
         <v>10000</v>
       </c>
-      <c r="F88" s="9" t="s">
+      <c r="F88" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9" t="s">
+      <c r="G88" s="8"/>
+      <c r="H88" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="I88" s="9" t="s">
+      <c r="I88" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J88" s="9" t="s">
+      <c r="J88" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="K88" s="9" t="s">
+      <c r="K88" s="8" t="s">
         <v>443</v>
       </c>
       <c r="L88" s="3"/>
@@ -9005,29 +9007,29 @@
       <c r="B89" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="8">
         <v>4</v>
       </c>
-      <c r="D89" s="9">
-        <v>1</v>
-      </c>
-      <c r="E89" s="9">
+      <c r="D89" s="8">
+        <v>1</v>
+      </c>
+      <c r="E89" s="8">
         <v>10000</v>
       </c>
-      <c r="F89" s="9" t="s">
+      <c r="F89" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="G89" s="9"/>
-      <c r="H89" s="9" t="s">
+      <c r="G89" s="8"/>
+      <c r="H89" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="I89" s="9" t="s">
+      <c r="I89" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="J89" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K89" s="9"/>
+      <c r="J89" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K89" s="8"/>
       <c r="L89" s="3"/>
       <c r="M89" s="3" t="s">
         <v>692</v>
@@ -9038,16 +9040,16 @@
       <c r="A90" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="7" t="s">
         <v>893</v>
       </c>
-      <c r="C90" s="8">
+      <c r="C90" s="7">
         <v>4</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D90" s="7">
         <v>3</v>
       </c>
-      <c r="E90" s="8">
+      <c r="E90" s="7">
         <v>250</v>
       </c>
       <c r="F90" s="3" t="s">
@@ -9081,31 +9083,31 @@
       <c r="B91" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="8">
         <v>2</v>
       </c>
-      <c r="D91" s="9">
-        <v>1</v>
-      </c>
-      <c r="E91" s="9">
+      <c r="D91" s="8">
+        <v>1</v>
+      </c>
+      <c r="E91" s="8">
         <v>10000</v>
       </c>
-      <c r="F91" s="9" t="s">
+      <c r="F91" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="G91" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H91" s="9" t="s">
+      <c r="H91" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I91" s="9" t="s">
+      <c r="I91" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="J91" s="9" t="s">
+      <c r="J91" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K91" s="9"/>
+      <c r="K91" s="8"/>
       <c r="L91" s="3"/>
       <c r="M91" s="3" t="s">
         <v>637</v>
@@ -9119,31 +9121,31 @@
       <c r="B92" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="8">
         <v>3</v>
       </c>
-      <c r="D92" s="9">
-        <v>1</v>
-      </c>
-      <c r="E92" s="9">
+      <c r="D92" s="8">
+        <v>1</v>
+      </c>
+      <c r="E92" s="8">
         <v>10000</v>
       </c>
-      <c r="F92" s="9" t="s">
+      <c r="F92" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G92" s="9" t="s">
+      <c r="G92" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H92" s="9" t="s">
+      <c r="H92" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="I92" s="9" t="s">
+      <c r="I92" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="J92" s="9" t="s">
+      <c r="J92" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K92" s="9"/>
+      <c r="K92" s="8"/>
       <c r="L92" s="3"/>
       <c r="M92" s="3" t="s">
         <v>740</v>
@@ -9157,29 +9159,29 @@
       <c r="B93" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="8">
         <v>4</v>
       </c>
-      <c r="D93" s="9">
-        <v>1</v>
-      </c>
-      <c r="E93" s="9">
+      <c r="D93" s="8">
+        <v>1</v>
+      </c>
+      <c r="E93" s="8">
         <v>10000</v>
       </c>
-      <c r="F93" s="9" t="s">
+      <c r="F93" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9" t="s">
+      <c r="G93" s="8"/>
+      <c r="H93" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="I93" s="9" t="s">
+      <c r="I93" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="J93" s="9" t="s">
+      <c r="J93" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="K93" s="9" t="s">
+      <c r="K93" s="8" t="s">
         <v>441</v>
       </c>
       <c r="L93" s="3"/>
@@ -9195,29 +9197,29 @@
       <c r="B94" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <v>4</v>
       </c>
-      <c r="D94" s="9">
-        <v>1</v>
-      </c>
-      <c r="E94" s="9">
+      <c r="D94" s="8">
+        <v>1</v>
+      </c>
+      <c r="E94" s="8">
         <v>10000</v>
       </c>
-      <c r="F94" s="9" t="s">
+      <c r="F94" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G94" s="9"/>
-      <c r="H94" s="9" t="s">
+      <c r="G94" s="8"/>
+      <c r="H94" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I94" s="9" t="s">
+      <c r="I94" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="J94" s="9" t="s">
+      <c r="J94" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K94" s="9" t="s">
+      <c r="K94" s="8" t="s">
         <v>452</v>
       </c>
       <c r="L94" s="3"/>
@@ -9233,29 +9235,29 @@
       <c r="B95" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="C95" s="9">
-        <v>1</v>
-      </c>
-      <c r="D95" s="9">
+      <c r="C95" s="8">
+        <v>1</v>
+      </c>
+      <c r="D95" s="8">
         <v>4</v>
       </c>
-      <c r="E95" s="9">
+      <c r="E95" s="8">
         <v>50</v>
       </c>
-      <c r="F95" s="9" t="s">
+      <c r="F95" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9" t="s">
+      <c r="G95" s="8"/>
+      <c r="H95" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I95" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J95" s="9" t="s">
+      <c r="I95" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J95" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="K95" s="9"/>
+      <c r="K95" s="8"/>
       <c r="L95" s="3"/>
       <c r="M95" s="3" t="s">
         <v>637</v>
@@ -9266,16 +9268,16 @@
       <c r="A96" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="7" t="s">
         <v>891</v>
       </c>
-      <c r="C96" s="8">
-        <v>1</v>
-      </c>
-      <c r="D96" s="8">
-        <v>1</v>
-      </c>
-      <c r="E96" s="8">
+      <c r="C96" s="7">
+        <v>1</v>
+      </c>
+      <c r="D96" s="7">
+        <v>1</v>
+      </c>
+      <c r="E96" s="7">
         <v>10000</v>
       </c>
       <c r="F96" s="3" t="s">
@@ -9305,29 +9307,29 @@
       <c r="B97" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="8">
         <v>2</v>
       </c>
-      <c r="D97" s="9">
-        <v>1</v>
-      </c>
-      <c r="E97" s="9">
+      <c r="D97" s="8">
+        <v>1</v>
+      </c>
+      <c r="E97" s="8">
         <v>10000</v>
       </c>
-      <c r="F97" s="9" t="s">
+      <c r="F97" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9" t="s">
+      <c r="G97" s="8"/>
+      <c r="H97" s="8" t="s">
         <v>906</v>
       </c>
-      <c r="I97" s="9" t="s">
+      <c r="I97" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="J97" s="9" t="s">
+      <c r="J97" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K97" s="9"/>
+      <c r="K97" s="8"/>
       <c r="L97" s="3"/>
       <c r="M97" s="3" t="s">
         <v>744</v>
@@ -9340,29 +9342,29 @@
       <c r="B98" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="C98" s="9">
+      <c r="C98" s="8">
         <v>2</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="8">
         <v>4</v>
       </c>
-      <c r="E98" s="9">
+      <c r="E98" s="8">
         <v>50</v>
       </c>
-      <c r="F98" s="9" t="s">
+      <c r="F98" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9" t="s">
+      <c r="G98" s="8"/>
+      <c r="H98" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I98" s="9" t="s">
+      <c r="I98" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="J98" s="9" t="s">
+      <c r="J98" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="K98" s="9"/>
+      <c r="K98" s="8"/>
       <c r="L98" s="3"/>
       <c r="M98" s="3" t="s">
         <v>713</v>
@@ -9378,29 +9380,29 @@
       <c r="B99" s="3" t="s">
         <v>750</v>
       </c>
-      <c r="C99" s="9">
+      <c r="C99" s="8">
         <v>2</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="8">
         <v>4</v>
       </c>
-      <c r="E99" s="9">
+      <c r="E99" s="8">
         <v>50</v>
       </c>
-      <c r="F99" s="9" t="s">
+      <c r="F99" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9" t="s">
+      <c r="G99" s="8"/>
+      <c r="H99" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I99" s="9" t="s">
+      <c r="I99" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="J99" s="9" t="s">
+      <c r="J99" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="K99" s="9"/>
+      <c r="K99" s="8"/>
       <c r="L99" s="3"/>
       <c r="M99" s="3" t="s">
         <v>713</v>
@@ -9413,29 +9415,29 @@
       <c r="B100" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="8">
         <v>2</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="8">
         <v>4</v>
       </c>
-      <c r="E100" s="9">
+      <c r="E100" s="8">
         <v>50</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F100" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9" t="s">
+      <c r="G100" s="8"/>
+      <c r="H100" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I100" s="9" t="s">
+      <c r="I100" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="J100" s="9" t="s">
+      <c r="J100" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="K100" s="9"/>
+      <c r="K100" s="8"/>
       <c r="L100" s="3"/>
       <c r="M100" s="3" t="s">
         <v>713</v>
@@ -9448,29 +9450,29 @@
       <c r="B101" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="8">
         <v>2</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="8">
         <v>4</v>
       </c>
-      <c r="E101" s="9">
+      <c r="E101" s="8">
         <v>50</v>
       </c>
-      <c r="F101" s="9" t="s">
+      <c r="F101" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9" t="s">
+      <c r="G101" s="8"/>
+      <c r="H101" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I101" s="9" t="s">
+      <c r="I101" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="J101" s="9" t="s">
+      <c r="J101" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="K101" s="9"/>
+      <c r="K101" s="8"/>
       <c r="L101" s="3"/>
       <c r="M101" s="3" t="s">
         <v>713</v>
@@ -9483,29 +9485,29 @@
       <c r="B102" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="8">
         <v>2</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="8">
         <v>2</v>
       </c>
-      <c r="E102" s="9">
+      <c r="E102" s="8">
         <v>2500</v>
       </c>
-      <c r="F102" s="9" t="s">
+      <c r="F102" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9" t="s">
+      <c r="G102" s="8"/>
+      <c r="H102" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I102" s="9" t="s">
+      <c r="I102" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J102" s="9" t="s">
+      <c r="J102" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="K102" s="9"/>
+      <c r="K102" s="8"/>
       <c r="L102" s="3"/>
       <c r="M102" s="3" t="s">
         <v>720</v>
@@ -9515,16 +9517,16 @@
       <c r="A103" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="7" t="s">
         <v>901</v>
       </c>
-      <c r="C103" s="8">
+      <c r="C103" s="7">
         <v>2</v>
       </c>
-      <c r="D103" s="8">
+      <c r="D103" s="7">
         <v>4</v>
       </c>
-      <c r="E103" s="8">
+      <c r="E103" s="7">
         <v>50</v>
       </c>
       <c r="F103" s="3" t="s">
@@ -9557,29 +9559,29 @@
       <c r="B104" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="8">
         <v>3</v>
       </c>
-      <c r="D104" s="9">
-        <v>1</v>
-      </c>
-      <c r="E104" s="9">
+      <c r="D104" s="8">
+        <v>1</v>
+      </c>
+      <c r="E104" s="8">
         <v>10000</v>
       </c>
-      <c r="F104" s="9" t="s">
+      <c r="F104" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9" t="s">
+      <c r="G104" s="8"/>
+      <c r="H104" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I104" s="9" t="s">
+      <c r="I104" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="J104" s="9" t="s">
+      <c r="J104" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="K104" s="9"/>
+      <c r="K104" s="8"/>
       <c r="L104" s="3"/>
       <c r="M104" s="3" t="s">
         <v>709</v>
@@ -9592,29 +9594,29 @@
       <c r="B105" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="C105" s="9">
+      <c r="C105" s="8">
         <v>4</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="8">
         <v>4</v>
       </c>
-      <c r="E105" s="9">
+      <c r="E105" s="8">
         <v>50</v>
       </c>
-      <c r="F105" s="9" t="s">
+      <c r="F105" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G105" s="9"/>
-      <c r="H105" s="9" t="s">
+      <c r="G105" s="8"/>
+      <c r="H105" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="I105" s="9" t="s">
+      <c r="I105" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="J105" s="9" t="s">
+      <c r="J105" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="K105" s="9"/>
+      <c r="K105" s="8"/>
       <c r="L105" s="3"/>
       <c r="M105" s="3" t="s">
         <v>661</v>
@@ -9624,16 +9626,16 @@
       <c r="A106" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="B106" s="7" t="s">
         <v>897</v>
       </c>
-      <c r="C106" s="8">
+      <c r="C106" s="7">
         <v>4</v>
       </c>
-      <c r="D106" s="8">
+      <c r="D106" s="7">
         <v>4</v>
       </c>
-      <c r="E106" s="8">
+      <c r="E106" s="7">
         <v>50</v>
       </c>
       <c r="F106" s="3" t="s">
@@ -9662,29 +9664,29 @@
       <c r="B107" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C107" s="8">
         <v>5</v>
       </c>
-      <c r="D107" s="9">
-        <v>1</v>
-      </c>
-      <c r="E107" s="9">
+      <c r="D107" s="8">
+        <v>1</v>
+      </c>
+      <c r="E107" s="8">
         <v>10000</v>
       </c>
-      <c r="F107" s="9" t="s">
+      <c r="F107" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="G107" s="9" t="s">
+      <c r="G107" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="H107" s="9" t="s">
+      <c r="H107" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="I107" s="9" t="s">
+      <c r="I107" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
+      <c r="J107" s="8"/>
+      <c r="K107" s="8"/>
       <c r="L107" s="3"/>
       <c r="M107" s="3" t="s">
         <v>624</v>
@@ -9837,27 +9839,27 @@
       <c r="B112" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="C112" s="9">
+      <c r="C112" s="8">
         <v>3</v>
       </c>
-      <c r="D112" s="9">
-        <v>1</v>
-      </c>
-      <c r="E112" s="9">
+      <c r="D112" s="8">
+        <v>1</v>
+      </c>
+      <c r="E112" s="8">
         <v>10000</v>
       </c>
-      <c r="F112" s="9" t="s">
+      <c r="F112" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G112" s="9"/>
-      <c r="H112" s="9" t="s">
+      <c r="G112" s="8"/>
+      <c r="H112" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I112" s="9" t="s">
+      <c r="I112" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J112" s="9"/>
-      <c r="K112" s="9"/>
+      <c r="J112" s="8"/>
+      <c r="K112" s="8"/>
       <c r="L112" s="3"/>
       <c r="M112" s="3" t="s">
         <v>670</v>
@@ -10191,16 +10193,16 @@
       <c r="A122" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="B122" s="9" t="s">
+      <c r="B122" s="8" t="s">
         <v>846</v>
       </c>
-      <c r="C122" s="8">
+      <c r="C122" s="7">
         <v>3</v>
       </c>
-      <c r="D122" s="9">
-        <v>1</v>
-      </c>
-      <c r="E122" s="9">
+      <c r="D122" s="8">
+        <v>1</v>
+      </c>
+      <c r="E122" s="8">
         <v>10000</v>
       </c>
       <c r="F122" s="3" t="s">
@@ -10226,16 +10228,16 @@
       <c r="A123" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="B123" s="9" t="s">
+      <c r="B123" s="8" t="s">
         <v>847</v>
       </c>
-      <c r="C123" s="8">
+      <c r="C123" s="7">
         <v>3</v>
       </c>
-      <c r="D123" s="9">
-        <v>1</v>
-      </c>
-      <c r="E123" s="9">
+      <c r="D123" s="8">
+        <v>1</v>
+      </c>
+      <c r="E123" s="8">
         <v>10000</v>
       </c>
       <c r="F123" s="3" t="s">
@@ -10261,16 +10263,16 @@
       <c r="A124" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="B124" s="8" t="s">
         <v>848</v>
       </c>
-      <c r="C124" s="8">
+      <c r="C124" s="7">
         <v>3</v>
       </c>
-      <c r="D124" s="9">
-        <v>1</v>
-      </c>
-      <c r="E124" s="9">
+      <c r="D124" s="8">
+        <v>1</v>
+      </c>
+      <c r="E124" s="8">
         <v>10000</v>
       </c>
       <c r="F124" s="3" t="s">
@@ -10438,16 +10440,16 @@
       <c r="A129" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="B129" s="7" t="s">
         <v>776</v>
       </c>
-      <c r="C129" s="8">
-        <v>1</v>
-      </c>
-      <c r="D129" s="8">
-        <v>1</v>
-      </c>
-      <c r="E129" s="8">
+      <c r="C129" s="7">
+        <v>1</v>
+      </c>
+      <c r="D129" s="7">
+        <v>1</v>
+      </c>
+      <c r="E129" s="7">
         <v>10000</v>
       </c>
       <c r="F129" s="3" t="s">
@@ -10473,16 +10475,16 @@
       <c r="A130" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B130" s="7" t="s">
         <v>781</v>
       </c>
-      <c r="C130" s="8">
-        <v>1</v>
-      </c>
-      <c r="D130" s="8">
-        <v>1</v>
-      </c>
-      <c r="E130" s="8">
+      <c r="C130" s="7">
+        <v>1</v>
+      </c>
+      <c r="D130" s="7">
+        <v>1</v>
+      </c>
+      <c r="E130" s="7">
         <v>10000</v>
       </c>
       <c r="F130" s="3" t="s">
@@ -10506,16 +10508,16 @@
       <c r="A131" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B131" s="8" t="s">
         <v>849</v>
       </c>
-      <c r="C131" s="8">
+      <c r="C131" s="7">
         <v>2</v>
       </c>
-      <c r="D131" s="9">
-        <v>1</v>
-      </c>
-      <c r="E131" s="9">
+      <c r="D131" s="8">
+        <v>1</v>
+      </c>
+      <c r="E131" s="8">
         <v>10000</v>
       </c>
       <c r="F131" s="3" t="s">
@@ -10545,16 +10547,16 @@
       <c r="A132" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B132" s="8" t="s">
+      <c r="B132" s="7" t="s">
         <v>774</v>
       </c>
-      <c r="C132" s="8">
+      <c r="C132" s="7">
         <v>3</v>
       </c>
-      <c r="D132" s="8">
-        <v>1</v>
-      </c>
-      <c r="E132" s="8">
+      <c r="D132" s="7">
+        <v>1</v>
+      </c>
+      <c r="E132" s="7">
         <v>10000</v>
       </c>
       <c r="F132" s="3" t="s">
@@ -10578,16 +10580,16 @@
       <c r="A133" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="B133" s="9" t="s">
+      <c r="B133" s="8" t="s">
         <v>850</v>
       </c>
-      <c r="C133" s="8">
+      <c r="C133" s="7">
         <v>3</v>
       </c>
-      <c r="D133" s="9">
-        <v>1</v>
-      </c>
-      <c r="E133" s="9">
+      <c r="D133" s="8">
+        <v>1</v>
+      </c>
+      <c r="E133" s="8">
         <v>10000</v>
       </c>
       <c r="F133" s="3" t="s">
@@ -10615,16 +10617,16 @@
       <c r="A134" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="C134" s="8">
+      <c r="C134" s="7">
         <v>4</v>
       </c>
-      <c r="D134" s="8">
+      <c r="D134" s="7">
         <v>4</v>
       </c>
-      <c r="E134" s="8">
+      <c r="E134" s="7">
         <v>50</v>
       </c>
       <c r="F134" s="3" t="s">
@@ -10650,16 +10652,16 @@
       <c r="A135" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="C135" s="8">
+      <c r="C135" s="7">
         <v>4</v>
       </c>
-      <c r="D135" s="8">
+      <c r="D135" s="7">
         <v>4</v>
       </c>
-      <c r="E135" s="8">
+      <c r="E135" s="7">
         <v>50</v>
       </c>
       <c r="F135" s="3" t="s">
@@ -10685,16 +10687,16 @@
       <c r="A136" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B136" s="8" t="s">
+      <c r="B136" s="7" t="s">
         <v>779</v>
       </c>
-      <c r="C136" s="8">
+      <c r="C136" s="7">
         <v>4</v>
       </c>
-      <c r="D136" s="8">
+      <c r="D136" s="7">
         <v>4</v>
       </c>
-      <c r="E136" s="8">
+      <c r="E136" s="7">
         <v>50</v>
       </c>
       <c r="F136" s="3" t="s">
@@ -10720,16 +10722,16 @@
       <c r="A137" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="B137" s="8" t="s">
+      <c r="B137" s="7" t="s">
         <v>780</v>
       </c>
-      <c r="C137" s="8">
+      <c r="C137" s="7">
         <v>4</v>
       </c>
-      <c r="D137" s="8">
+      <c r="D137" s="7">
         <v>4</v>
       </c>
-      <c r="E137" s="8">
+      <c r="E137" s="7">
         <v>50</v>
       </c>
       <c r="F137" s="3" t="s">
@@ -10755,16 +10757,16 @@
       <c r="A138" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="B138" s="9" t="s">
+      <c r="B138" s="8" t="s">
         <v>907</v>
       </c>
-      <c r="C138" s="9">
+      <c r="C138" s="8">
         <v>5</v>
       </c>
-      <c r="D138" s="9">
+      <c r="D138" s="8">
         <v>4</v>
       </c>
-      <c r="E138" s="9">
+      <c r="E138" s="8">
         <v>50</v>
       </c>
       <c r="F138" s="4" t="s">
@@ -10794,16 +10796,16 @@
       <c r="A139" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="B139" s="9" t="s">
+      <c r="B139" s="8" t="s">
         <v>908</v>
       </c>
-      <c r="C139" s="9">
+      <c r="C139" s="8">
         <v>5</v>
       </c>
-      <c r="D139" s="9">
+      <c r="D139" s="8">
         <v>4</v>
       </c>
-      <c r="E139" s="9">
+      <c r="E139" s="8">
         <v>50</v>
       </c>
       <c r="F139" s="4" t="s">
@@ -10833,16 +10835,16 @@
       <c r="A140" s="4" t="s">
         <v>843</v>
       </c>
-      <c r="B140" s="9" t="s">
+      <c r="B140" s="8" t="s">
         <v>844</v>
       </c>
-      <c r="C140" s="8">
+      <c r="C140" s="7">
         <v>2</v>
       </c>
-      <c r="D140" s="9">
-        <v>1</v>
-      </c>
-      <c r="E140" s="9">
+      <c r="D140" s="8">
+        <v>1</v>
+      </c>
+      <c r="E140" s="8">
         <v>10000</v>
       </c>
       <c r="F140" s="3" t="s">
@@ -10868,16 +10870,16 @@
       <c r="A141" s="4" t="s">
         <v>843</v>
       </c>
-      <c r="B141" s="9" t="s">
+      <c r="B141" s="8" t="s">
         <v>841</v>
       </c>
-      <c r="C141" s="8">
+      <c r="C141" s="7">
         <v>4</v>
       </c>
-      <c r="D141" s="9">
-        <v>1</v>
-      </c>
-      <c r="E141" s="9">
+      <c r="D141" s="8">
+        <v>1</v>
+      </c>
+      <c r="E141" s="8">
         <v>10000</v>
       </c>
       <c r="F141" s="3" t="s">
@@ -10903,16 +10905,16 @@
       <c r="A142" s="4" t="s">
         <v>919</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B142" s="8" t="s">
         <v>927</v>
       </c>
-      <c r="C142" s="9">
+      <c r="C142" s="8">
         <v>4</v>
       </c>
-      <c r="D142" s="9">
+      <c r="D142" s="8">
         <v>3</v>
       </c>
-      <c r="E142" s="9">
+      <c r="E142" s="8">
         <v>250</v>
       </c>
       <c r="F142" s="4" t="s">
@@ -10938,16 +10940,16 @@
       <c r="A143" s="4" t="s">
         <v>919</v>
       </c>
-      <c r="B143" s="9" t="s">
+      <c r="B143" s="8" t="s">
         <v>924</v>
       </c>
-      <c r="C143" s="9">
-        <v>1</v>
-      </c>
-      <c r="D143" s="9">
-        <v>1</v>
-      </c>
-      <c r="E143" s="9">
+      <c r="C143" s="8">
+        <v>1</v>
+      </c>
+      <c r="D143" s="8">
+        <v>1</v>
+      </c>
+      <c r="E143" s="8">
         <v>10000</v>
       </c>
       <c r="F143" s="4" t="s">
@@ -10973,10 +10975,10 @@
       <c r="A144" s="4" t="s">
         <v>919</v>
       </c>
-      <c r="B144" s="9" t="s">
+      <c r="B144" s="8" t="s">
         <v>925</v>
       </c>
-      <c r="C144" s="9">
+      <c r="C144" s="8">
         <v>3</v>
       </c>
       <c r="D144" s="3">
@@ -11010,16 +11012,16 @@
       <c r="A145" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="B145" s="9" t="s">
+      <c r="B145" s="8" t="s">
         <v>922</v>
       </c>
       <c r="C145" s="3">
         <v>1</v>
       </c>
-      <c r="D145" s="9">
-        <v>1</v>
-      </c>
-      <c r="E145" s="9">
+      <c r="D145" s="8">
+        <v>1</v>
+      </c>
+      <c r="E145" s="8">
         <v>10000</v>
       </c>
       <c r="F145" s="4" t="s">
@@ -11043,16 +11045,16 @@
       <c r="A146" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="B146" s="9" t="s">
+      <c r="B146" s="8" t="s">
         <v>928</v>
       </c>
       <c r="C146" s="3">
         <v>2</v>
       </c>
-      <c r="D146" s="9">
+      <c r="D146" s="8">
         <v>2</v>
       </c>
-      <c r="E146" s="9">
+      <c r="E146" s="8">
         <v>2500</v>
       </c>
       <c r="F146" s="4" t="s">
@@ -11080,16 +11082,16 @@
       <c r="A147" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B147" s="8" t="s">
         <v>926</v>
       </c>
       <c r="C147" s="3">
         <v>3</v>
       </c>
-      <c r="D147" s="9">
+      <c r="D147" s="8">
         <v>2</v>
       </c>
-      <c r="E147" s="9">
+      <c r="E147" s="8">
         <v>2500</v>
       </c>
       <c r="F147" s="4" t="s">
@@ -11127,10 +11129,10 @@
       <c r="C148" s="3">
         <v>2</v>
       </c>
-      <c r="D148" s="9">
-        <v>1</v>
-      </c>
-      <c r="E148" s="9">
+      <c r="D148" s="8">
+        <v>1</v>
+      </c>
+      <c r="E148" s="8">
         <v>10000</v>
       </c>
       <c r="F148" s="4" t="s">
@@ -11155,39 +11157,83 @@
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
+      <c r="A149" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="3" t="s">
         <v>923</v>
       </c>
-      <c r="C149" s="2">
-        <v>1</v>
-      </c>
-      <c r="D149" s="10">
+      <c r="C149" s="3">
+        <v>1</v>
+      </c>
+      <c r="D149" s="8">
         <v>4</v>
       </c>
-      <c r="E149" s="10">
+      <c r="E149" s="8">
         <v>50</v>
       </c>
-      <c r="F149" s="5" t="s">
+      <c r="F149" s="4" t="s">
         <v>934</v>
       </c>
-      <c r="G149" s="2"/>
-      <c r="H149" s="5" t="s">
+      <c r="G149" s="3"/>
+      <c r="H149" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="I149" s="5" t="s">
+      <c r="I149" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J149" s="5" t="s">
+      <c r="J149" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K149" s="2"/>
-      <c r="L149" s="2"/>
-      <c r="M149" s="5" t="s">
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="4" t="s">
         <v>932</v>
       </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C150" s="10">
+        <v>10</v>
+      </c>
+      <c r="D150" s="2">
+        <v>1</v>
+      </c>
+      <c r="E150" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="I150" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J150" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="K150" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L150" s="2"/>
+      <c r="M150" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="8"/>
+      <c r="E151" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A143:E149">
@@ -11205,7 +11251,7 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
quest update + charm
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\Craft-to-Exile-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79039AC-22EF-42FD-AE8D-7DD106F07648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAD5C2A-7A51-44F4-A949-6981AA16839D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D4271B40-E291-4F7D-B212-DFF8B5827327}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="950">
   <si>
     <t>armor_percent</t>
   </si>
@@ -2843,6 +2843,48 @@
   </si>
   <si>
     <t>blaze_bow</t>
+  </si>
+  <si>
+    <t>gheeds_fortune</t>
+  </si>
+  <si>
+    <t>0.25 sta</t>
+  </si>
+  <si>
+    <t>0.5 sta</t>
+  </si>
+  <si>
+    <t>0.25 sta, 0.25 int</t>
+  </si>
+  <si>
+    <t>0.25 sta, 0.25 vit</t>
+  </si>
+  <si>
+    <t>0.25 sta, 0.25 dex</t>
+  </si>
+  <si>
+    <t>0.25 sta, 0.25 str</t>
+  </si>
+  <si>
+    <t>0.25 sta, 0.25 wis</t>
+  </si>
+  <si>
+    <t>hellfire_ocean</t>
+  </si>
+  <si>
+    <t>hellfire_fire</t>
+  </si>
+  <si>
+    <t>hellfire_storm</t>
+  </si>
+  <si>
+    <t>hellfire_nature</t>
+  </si>
+  <si>
+    <t>hellfire_hunting</t>
+  </si>
+  <si>
+    <t>hellfire_divine</t>
   </si>
 </sst>
 </file>
@@ -2914,7 +2956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2925,7 +2967,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5827,10 +5870,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:N151"/>
+  <dimension ref="A1:N157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="G149" sqref="G149"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="M146" sqref="M146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6681,7 +6724,7 @@
         <v>655</v>
       </c>
       <c r="C24" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -6716,7 +6759,7 @@
         <v>656</v>
       </c>
       <c r="C25" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -6751,7 +6794,7 @@
         <v>657</v>
       </c>
       <c r="C26" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -6788,7 +6831,7 @@
         <v>658</v>
       </c>
       <c r="C27" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -11192,48 +11235,284 @@
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" s="3" t="s">
         <v>935</v>
       </c>
-      <c r="C150" s="10">
+      <c r="C150" s="7">
         <v>10</v>
       </c>
-      <c r="D150" s="2">
-        <v>1</v>
-      </c>
-      <c r="E150" s="2">
+      <c r="D150" s="3">
+        <v>1</v>
+      </c>
+      <c r="E150" s="3">
         <v>10000</v>
       </c>
-      <c r="F150" s="2" t="s">
+      <c r="F150" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2" t="s">
+      <c r="G150" s="3"/>
+      <c r="H150" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="I150" s="2" t="s">
+      <c r="I150" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J150" s="2" t="s">
+      <c r="J150" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="K150" s="2" t="s">
+      <c r="K150" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L150" s="2"/>
-      <c r="M150" s="2" t="s">
+      <c r="L150" s="3"/>
+      <c r="M150" s="3" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="8"/>
+      <c r="A151" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="C151" s="4">
+        <v>3</v>
+      </c>
+      <c r="D151" s="8">
+        <v>2</v>
+      </c>
+      <c r="E151" s="8">
+        <v>2500</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G151" s="3"/>
+      <c r="H151" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="J151" s="3"/>
+      <c r="K151" s="3"/>
+      <c r="L151" s="3"/>
+      <c r="M151" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="C152" s="4">
+        <v>4</v>
+      </c>
+      <c r="D152" s="8">
+        <v>3</v>
+      </c>
+      <c r="E152" s="8">
+        <v>250</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="G152" s="3"/>
+      <c r="H152" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K152" s="3"/>
+      <c r="L152" s="3"/>
+      <c r="M152" s="4" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="C153" s="4">
+        <v>4</v>
+      </c>
+      <c r="D153" s="8">
+        <v>3</v>
+      </c>
+      <c r="E153" s="8">
+        <v>250</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="G153" s="3"/>
+      <c r="H153" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K153" s="3"/>
+      <c r="L153" s="3"/>
+      <c r="M153" s="4" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="C154" s="4">
+        <v>4</v>
+      </c>
+      <c r="D154" s="8">
+        <v>3</v>
+      </c>
+      <c r="E154" s="8">
+        <v>250</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="G154" s="3"/>
+      <c r="H154" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="4" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="C155" s="4">
+        <v>4</v>
+      </c>
+      <c r="D155" s="8">
+        <v>3</v>
+      </c>
+      <c r="E155" s="8">
+        <v>250</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="G155" s="3"/>
+      <c r="H155" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K155" s="3"/>
+      <c r="L155" s="3"/>
+      <c r="M155" s="4" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="C156" s="4">
+        <v>4</v>
+      </c>
+      <c r="D156" s="8">
+        <v>3</v>
+      </c>
+      <c r="E156" s="8">
+        <v>250</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="G156" s="3"/>
+      <c r="H156" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K156" s="3"/>
+      <c r="L156" s="3"/>
+      <c r="M156" s="4" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>949</v>
+      </c>
+      <c r="C157" s="10">
+        <v>4</v>
+      </c>
+      <c r="D157" s="11">
+        <v>3</v>
+      </c>
+      <c r="E157" s="11">
+        <v>250</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="G157" s="2"/>
+      <c r="H157" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I157" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="J157" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K157" s="2"/>
+      <c r="L157" s="2"/>
+      <c r="M157" s="10" t="s">
+        <v>940</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A143:E149">
@@ -11251,8 +11530,8 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>